<commit_message>
update triger answer display sample value
</commit_message>
<xml_diff>
--- a/weightModeCMD.xlsx
+++ b/weightModeCMD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\GitWorkSpace\WeightModeGit\screen_firmware\WeightMode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9270864-733F-4609-84DE-A1429A17A27B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059DC77B-59EE-4AED-9D29-785FB7BA5C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1320" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="预览模式" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
   <si>
     <t>背景色</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -455,12 +455,48 @@
 1-8：单一对应通道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SDWE-&gt;MCU
+MCU-&gt;SDWE
+(点采样值)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1#通道实时值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2#通道实时值</t>
+  </si>
+  <si>
+    <t>3#通道实时值</t>
+  </si>
+  <si>
+    <t>4#通道实时值</t>
+  </si>
+  <si>
+    <t>5#通道实时值</t>
+  </si>
+  <si>
+    <t>6#通道实时值</t>
+  </si>
+  <si>
+    <t>7#通道实时值</t>
+  </si>
+  <si>
+    <t>8#通道实时值</t>
+  </si>
+  <si>
+    <t>校准时：
+发送每个通道值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +512,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
@@ -521,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -630,11 +674,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -669,6 +750,12 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -678,10 +765,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,8 +780,26 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,17 +1133,17 @@
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1176,19 +1281,19 @@
       <c r="A2">
         <v>60</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1338,7 +1443,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -1851,11 +1956,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE25038-9FB6-4DB7-BF7A-8C3715897DB9}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -1870,10 +1975,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="15" t="s">
         <v>43</v>
       </c>
@@ -1901,10 +2006,10 @@
       <c r="D2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1922,8 +2027,8 @@
       <c r="D3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="22"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
@@ -1939,8 +2044,8 @@
       <c r="D4" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
@@ -1956,8 +2061,8 @@
       <c r="D5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -1973,8 +2078,8 @@
       <c r="D6" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
@@ -1990,8 +2095,8 @@
       <c r="D7" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
@@ -2007,8 +2112,8 @@
       <c r="D8" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="22"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
@@ -2024,8 +2129,8 @@
       <c r="D9" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -2041,10 +2146,10 @@
       <c r="D10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="23" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2062,8 +2167,8 @@
       <c r="D11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -2079,8 +2184,8 @@
       <c r="D12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
@@ -2096,8 +2201,8 @@
       <c r="D13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
@@ -2113,8 +2218,8 @@
       <c r="D14" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
@@ -2130,8 +2235,8 @@
       <c r="D15" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -2147,8 +2252,8 @@
       <c r="D16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
@@ -2164,8 +2269,8 @@
       <c r="D17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
@@ -2181,10 +2286,10 @@
       <c r="D18" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="23" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2202,8 +2307,8 @@
       <c r="D19" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
@@ -2219,8 +2324,8 @@
       <c r="D20" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="22"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
@@ -2236,8 +2341,8 @@
       <c r="D21" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="22"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
@@ -2253,8 +2358,8 @@
       <c r="D22" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
@@ -2270,8 +2375,8 @@
       <c r="D23" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
@@ -2287,8 +2392,8 @@
       <c r="D24" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="22"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
@@ -2304,8 +2409,8 @@
       <c r="D25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="22"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="27" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
@@ -2321,7 +2426,7 @@
       <c r="D27" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="19" t="s">
         <v>118</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -2345,7 +2450,7 @@
       <c r="E28" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="23" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2366,7 +2471,7 @@
       <c r="E29" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="22"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
@@ -2385,7 +2490,7 @@
       <c r="E30" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="22"/>
+      <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
@@ -2404,7 +2509,7 @@
       <c r="E31" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="22"/>
+      <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
@@ -2423,7 +2528,7 @@
       <c r="E32" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
@@ -2442,7 +2547,7 @@
       <c r="E33" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
@@ -2461,7 +2566,7 @@
       <c r="E34" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="22"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
@@ -2480,7 +2585,7 @@
       <c r="E35" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="22"/>
+      <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
@@ -2499,7 +2604,7 @@
       <c r="E36" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F36" s="22"/>
+      <c r="F36" s="23"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
@@ -2518,7 +2623,7 @@
       <c r="E37" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
@@ -2534,10 +2639,10 @@
       <c r="D38" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="23" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2555,8 +2660,8 @@
       <c r="D39" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="22"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
@@ -2572,8 +2677,8 @@
       <c r="D40" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
@@ -2589,8 +2694,8 @@
       <c r="D41" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
@@ -2606,8 +2711,8 @@
       <c r="D42" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
@@ -2623,8 +2728,8 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
@@ -2640,8 +2745,8 @@
       <c r="D44" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="22"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="23"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
@@ -2657,8 +2762,8 @@
       <c r="D45" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="22"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="23"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
@@ -2674,8 +2779,8 @@
       <c r="D46" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="22"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
@@ -2691,8 +2796,8 @@
       <c r="D47" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="22"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
@@ -2708,11 +2813,11 @@
       <c r="D48" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F48" s="22" t="s">
-        <v>116</v>
+      <c r="F48" s="28" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2729,8 +2834,8 @@
       <c r="D49" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="21"/>
-      <c r="F49" s="22"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
@@ -2746,8 +2851,8 @@
       <c r="D50" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="22"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
@@ -2763,8 +2868,8 @@
       <c r="D51" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="21"/>
-      <c r="F51" s="22"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
@@ -2780,8 +2885,8 @@
       <c r="D52" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="E52" s="21"/>
-      <c r="F52" s="22"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -2797,8 +2902,8 @@
       <c r="D53" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E53" s="21"/>
-      <c r="F53" s="22"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
@@ -2814,8 +2919,8 @@
       <c r="D54" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E54" s="21"/>
-      <c r="F54" s="22"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
@@ -2831,8 +2936,8 @@
       <c r="D55" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="21"/>
-      <c r="F55" s="22"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="23"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
@@ -2848,8 +2953,8 @@
       <c r="D56" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="21"/>
-      <c r="F56" s="22"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
@@ -2865,23 +2970,165 @@
       <c r="D57" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="21"/>
-      <c r="F57" s="22"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="23"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
+        <v>542</v>
+      </c>
+      <c r="B58" s="18" t="str">
+        <f t="shared" ref="B58:B65" si="4">"0x"&amp;DEC2HEX(A58,4)</f>
+        <v>0x021E</v>
+      </c>
+      <c r="C58" s="18">
+        <v>1</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="18">
+        <v>543</v>
+      </c>
+      <c r="B59" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x021F</v>
+      </c>
+      <c r="C59" s="18">
+        <v>1</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" s="29"/>
+      <c r="F59" s="33"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="18">
+        <v>544</v>
+      </c>
+      <c r="B60" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0220</v>
+      </c>
+      <c r="C60" s="18">
+        <v>1</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E60" s="29"/>
+      <c r="F60" s="33"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="18">
+        <v>545</v>
+      </c>
+      <c r="B61" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0221</v>
+      </c>
+      <c r="C61" s="18">
+        <v>1</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" s="29"/>
+      <c r="F61" s="33"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="18">
+        <v>546</v>
+      </c>
+      <c r="B62" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0222</v>
+      </c>
+      <c r="C62" s="18">
+        <v>1</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E62" s="29"/>
+      <c r="F62" s="33"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="18">
+        <v>547</v>
+      </c>
+      <c r="B63" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0223</v>
+      </c>
+      <c r="C63" s="18">
+        <v>1</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E63" s="29"/>
+      <c r="F63" s="33"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="18">
+        <v>548</v>
+      </c>
+      <c r="B64" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0224</v>
+      </c>
+      <c r="C64" s="18">
+        <v>1</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E64" s="29"/>
+      <c r="F64" s="33"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="18">
+        <v>549</v>
+      </c>
+      <c r="B65" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0225</v>
+      </c>
+      <c r="C65" s="18">
+        <v>1</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" s="30"/>
+      <c r="F65" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="E58:E65"/>
+    <mergeCell ref="F58:F65"/>
+    <mergeCell ref="E48:E57"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="E2:E9"/>
     <mergeCell ref="F48:F57"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="F18:F25"/>
     <mergeCell ref="F28:F37"/>
     <mergeCell ref="F38:F47"/>
-    <mergeCell ref="E48:E57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="E10:E17"/>
-    <mergeCell ref="E38:E47"/>
-    <mergeCell ref="E2:E9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>